<commit_message>
Correctif orthographe "accueil" (#154)
Correctif orthographe "accueil" à la place de "acceuil" sur le nom de la slice.

Co-authored-by: TristanRiri <tristan.rieu@gmail.com> 6700c575748b0a4c9597e309011e280451c6d2d5
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-sdo-task.xlsx
+++ b/ig/main/StructureDefinition-sdo-task.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8539" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8539" uniqueCount="719">
   <si>
     <t>Property</t>
   </si>
@@ -1835,43 +1835,40 @@
     <t>https://mos.esante.gouv.fr/NOS/JDV_J34-CategorieOrganisation-ROR/FHIR/JDV-J34-CategorieOrganisation-ROR</t>
   </si>
   <si>
-    <t>Task.input:temporaliteAcceuil</t>
-  </si>
-  <si>
-    <t>temporaliteAcceuil</t>
+    <t>Task.input:temporaliteAccueil</t>
+  </si>
+  <si>
+    <t>temporaliteAccueil</t>
   </si>
   <si>
     <t>Permet de définir la fréquence d'accueil lors d'une prise en charge en ESMS</t>
   </si>
   <si>
-    <t>Task.input:temporaliteAcceuil.id</t>
-  </si>
-  <si>
-    <t>Task.input:temporaliteAcceuil.extension</t>
-  </si>
-  <si>
-    <t>Task.input:temporaliteAcceuil.modifierExtension</t>
-  </si>
-  <si>
-    <t>Task.input:temporaliteAcceuil.type</t>
-  </si>
-  <si>
-    <t>Task.input:temporaliteAcceuil.type.id</t>
-  </si>
-  <si>
-    <t>Task.input:temporaliteAcceuil.type.extension</t>
-  </si>
-  <si>
-    <t>Task.input:temporaliteAcceuil.type.coding</t>
-  </si>
-  <si>
-    <t>Task.input:temporaliteAcceuil.type.text</t>
-  </si>
-  <si>
-    <t>temporaliteAccueil</t>
-  </si>
-  <si>
-    <t>Task.input:temporaliteAcceuil.value[x]</t>
+    <t>Task.input:temporaliteAccueil.id</t>
+  </si>
+  <si>
+    <t>Task.input:temporaliteAccueil.extension</t>
+  </si>
+  <si>
+    <t>Task.input:temporaliteAccueil.modifierExtension</t>
+  </si>
+  <si>
+    <t>Task.input:temporaliteAccueil.type</t>
+  </si>
+  <si>
+    <t>Task.input:temporaliteAccueil.type.id</t>
+  </si>
+  <si>
+    <t>Task.input:temporaliteAccueil.type.extension</t>
+  </si>
+  <si>
+    <t>Task.input:temporaliteAccueil.type.coding</t>
+  </si>
+  <si>
+    <t>Task.input:temporaliteAccueil.type.text</t>
+  </si>
+  <si>
+    <t>Task.input:temporaliteAccueil.value[x]</t>
   </si>
   <si>
     <t>https://mos.esante.gouv.fr/NOS/JDV_J30-TemporaliteAccueil-ROR/FHIR/JDV-J30-TemporaliteAccueil-ROR</t>
@@ -19449,7 +19446,7 @@
       </c>
       <c r="Q148" s="2"/>
       <c r="R148" t="s" s="2">
-        <v>599</v>
+        <v>589</v>
       </c>
       <c r="S148" t="s" s="2">
         <v>76</v>
@@ -19520,7 +19517,7 @@
     </row>
     <row r="149">
       <c r="A149" t="s" s="2">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B149" t="s" s="2">
         <v>466</v>
@@ -19583,7 +19580,7 @@
       </c>
       <c r="Y149" s="2"/>
       <c r="Z149" t="s" s="2">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="AA149" t="s" s="2">
         <v>76</v>
@@ -19630,13 +19627,13 @@
     </row>
     <row r="150">
       <c r="A150" t="s" s="2">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B150" t="s" s="2">
         <v>448</v>
       </c>
       <c r="C150" t="s" s="2">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D150" t="s" s="2">
         <v>449</v>
@@ -19661,7 +19658,7 @@
         <v>418</v>
       </c>
       <c r="L150" t="s" s="2">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="M150" t="s" s="2">
         <v>452</v>
@@ -19746,7 +19743,7 @@
     </row>
     <row r="151">
       <c r="A151" t="s" s="2">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B151" t="s" s="2">
         <v>456</v>
@@ -19858,7 +19855,7 @@
     </row>
     <row r="152">
       <c r="A152" t="s" s="2">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B152" t="s" s="2">
         <v>457</v>
@@ -19972,7 +19969,7 @@
     </row>
     <row r="153">
       <c r="A153" t="s" s="2">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B153" t="s" s="2">
         <v>458</v>
@@ -20088,7 +20085,7 @@
     </row>
     <row r="154">
       <c r="A154" t="s" s="2">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B154" t="s" s="2">
         <v>459</v>
@@ -20204,7 +20201,7 @@
     </row>
     <row r="155">
       <c r="A155" t="s" s="2">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B155" t="s" s="2">
         <v>478</v>
@@ -20316,7 +20313,7 @@
     </row>
     <row r="156">
       <c r="A156" t="s" s="2">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B156" t="s" s="2">
         <v>480</v>
@@ -20430,7 +20427,7 @@
     </row>
     <row r="157">
       <c r="A157" t="s" s="2">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B157" t="s" s="2">
         <v>482</v>
@@ -20546,7 +20543,7 @@
     </row>
     <row r="158">
       <c r="A158" t="s" s="2">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B158" t="s" s="2">
         <v>491</v>
@@ -20591,7 +20588,7 @@
       </c>
       <c r="Q158" s="2"/>
       <c r="R158" t="s" s="2">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="S158" t="s" s="2">
         <v>76</v>
@@ -20662,7 +20659,7 @@
     </row>
     <row r="159">
       <c r="A159" t="s" s="2">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B159" t="s" s="2">
         <v>466</v>
@@ -20688,7 +20685,7 @@
         <v>76</v>
       </c>
       <c r="K159" t="s" s="2">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="L159" t="s" s="2">
         <v>468</v>
@@ -20774,13 +20771,13 @@
     </row>
     <row r="160">
       <c r="A160" t="s" s="2">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B160" t="s" s="2">
         <v>448</v>
       </c>
       <c r="C160" t="s" s="2">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D160" t="s" s="2">
         <v>449</v>
@@ -20805,7 +20802,7 @@
         <v>418</v>
       </c>
       <c r="L160" t="s" s="2">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="M160" t="s" s="2">
         <v>452</v>
@@ -20890,7 +20887,7 @@
     </row>
     <row r="161">
       <c r="A161" t="s" s="2">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B161" t="s" s="2">
         <v>456</v>
@@ -21002,7 +20999,7 @@
     </row>
     <row r="162">
       <c r="A162" t="s" s="2">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B162" t="s" s="2">
         <v>457</v>
@@ -21116,7 +21113,7 @@
     </row>
     <row r="163">
       <c r="A163" t="s" s="2">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B163" t="s" s="2">
         <v>458</v>
@@ -21232,7 +21229,7 @@
     </row>
     <row r="164">
       <c r="A164" t="s" s="2">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B164" t="s" s="2">
         <v>459</v>
@@ -21348,7 +21345,7 @@
     </row>
     <row r="165">
       <c r="A165" t="s" s="2">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B165" t="s" s="2">
         <v>478</v>
@@ -21460,7 +21457,7 @@
     </row>
     <row r="166">
       <c r="A166" t="s" s="2">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B166" t="s" s="2">
         <v>480</v>
@@ -21574,7 +21571,7 @@
     </row>
     <row r="167">
       <c r="A167" t="s" s="2">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B167" t="s" s="2">
         <v>482</v>
@@ -21690,7 +21687,7 @@
     </row>
     <row r="168">
       <c r="A168" t="s" s="2">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B168" t="s" s="2">
         <v>491</v>
@@ -21735,7 +21732,7 @@
       </c>
       <c r="Q168" s="2"/>
       <c r="R168" t="s" s="2">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="S168" t="s" s="2">
         <v>76</v>
@@ -21806,7 +21803,7 @@
     </row>
     <row r="169">
       <c r="A169" t="s" s="2">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B169" t="s" s="2">
         <v>466</v>
@@ -21869,7 +21866,7 @@
       </c>
       <c r="Y169" s="2"/>
       <c r="Z169" t="s" s="2">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="AA169" t="s" s="2">
         <v>76</v>
@@ -21916,13 +21913,13 @@
     </row>
     <row r="170">
       <c r="A170" t="s" s="2">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B170" t="s" s="2">
         <v>448</v>
       </c>
       <c r="C170" t="s" s="2">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D170" t="s" s="2">
         <v>449</v>
@@ -21947,7 +21944,7 @@
         <v>418</v>
       </c>
       <c r="L170" t="s" s="2">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="M170" t="s" s="2">
         <v>452</v>
@@ -22032,7 +22029,7 @@
     </row>
     <row r="171">
       <c r="A171" t="s" s="2">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B171" t="s" s="2">
         <v>456</v>
@@ -22144,7 +22141,7 @@
     </row>
     <row r="172">
       <c r="A172" t="s" s="2">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B172" t="s" s="2">
         <v>457</v>
@@ -22258,7 +22255,7 @@
     </row>
     <row r="173">
       <c r="A173" t="s" s="2">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B173" t="s" s="2">
         <v>458</v>
@@ -22374,7 +22371,7 @@
     </row>
     <row r="174">
       <c r="A174" t="s" s="2">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B174" t="s" s="2">
         <v>459</v>
@@ -22490,7 +22487,7 @@
     </row>
     <row r="175">
       <c r="A175" t="s" s="2">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B175" t="s" s="2">
         <v>478</v>
@@ -22602,7 +22599,7 @@
     </row>
     <row r="176">
       <c r="A176" t="s" s="2">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B176" t="s" s="2">
         <v>480</v>
@@ -22716,7 +22713,7 @@
     </row>
     <row r="177">
       <c r="A177" t="s" s="2">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B177" t="s" s="2">
         <v>482</v>
@@ -22832,7 +22829,7 @@
     </row>
     <row r="178">
       <c r="A178" t="s" s="2">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B178" t="s" s="2">
         <v>491</v>
@@ -22877,7 +22874,7 @@
       </c>
       <c r="Q178" s="2"/>
       <c r="R178" t="s" s="2">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="S178" t="s" s="2">
         <v>76</v>
@@ -22948,7 +22945,7 @@
     </row>
     <row r="179">
       <c r="A179" t="s" s="2">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B179" t="s" s="2">
         <v>466</v>
@@ -23011,7 +23008,7 @@
       </c>
       <c r="Y179" s="2"/>
       <c r="Z179" t="s" s="2">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="AA179" t="s" s="2">
         <v>76</v>
@@ -23058,13 +23055,13 @@
     </row>
     <row r="180">
       <c r="A180" t="s" s="2">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B180" t="s" s="2">
         <v>448</v>
       </c>
       <c r="C180" t="s" s="2">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D180" t="s" s="2">
         <v>449</v>
@@ -23089,7 +23086,7 @@
         <v>418</v>
       </c>
       <c r="L180" t="s" s="2">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="M180" t="s" s="2">
         <v>452</v>
@@ -23174,7 +23171,7 @@
     </row>
     <row r="181">
       <c r="A181" t="s" s="2">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B181" t="s" s="2">
         <v>456</v>
@@ -23286,7 +23283,7 @@
     </row>
     <row r="182">
       <c r="A182" t="s" s="2">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B182" t="s" s="2">
         <v>457</v>
@@ -23400,7 +23397,7 @@
     </row>
     <row r="183">
       <c r="A183" t="s" s="2">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B183" t="s" s="2">
         <v>458</v>
@@ -23516,7 +23513,7 @@
     </row>
     <row r="184">
       <c r="A184" t="s" s="2">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B184" t="s" s="2">
         <v>459</v>
@@ -23632,7 +23629,7 @@
     </row>
     <row r="185">
       <c r="A185" t="s" s="2">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B185" t="s" s="2">
         <v>478</v>
@@ -23744,7 +23741,7 @@
     </row>
     <row r="186">
       <c r="A186" t="s" s="2">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B186" t="s" s="2">
         <v>480</v>
@@ -23858,7 +23855,7 @@
     </row>
     <row r="187">
       <c r="A187" t="s" s="2">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B187" t="s" s="2">
         <v>482</v>
@@ -23974,7 +23971,7 @@
     </row>
     <row r="188">
       <c r="A188" t="s" s="2">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B188" t="s" s="2">
         <v>491</v>
@@ -24019,7 +24016,7 @@
       </c>
       <c r="Q188" s="2"/>
       <c r="R188" t="s" s="2">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="S188" t="s" s="2">
         <v>76</v>
@@ -24090,7 +24087,7 @@
     </row>
     <row r="189">
       <c r="A189" t="s" s="2">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B189" t="s" s="2">
         <v>466</v>
@@ -24202,13 +24199,13 @@
     </row>
     <row r="190">
       <c r="A190" t="s" s="2">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B190" t="s" s="2">
         <v>448</v>
       </c>
       <c r="C190" t="s" s="2">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D190" t="s" s="2">
         <v>449</v>
@@ -24233,7 +24230,7 @@
         <v>418</v>
       </c>
       <c r="L190" t="s" s="2">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="M190" t="s" s="2">
         <v>452</v>
@@ -24318,7 +24315,7 @@
     </row>
     <row r="191">
       <c r="A191" t="s" s="2">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B191" t="s" s="2">
         <v>456</v>
@@ -24430,7 +24427,7 @@
     </row>
     <row r="192">
       <c r="A192" t="s" s="2">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B192" t="s" s="2">
         <v>457</v>
@@ -24544,7 +24541,7 @@
     </row>
     <row r="193">
       <c r="A193" t="s" s="2">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B193" t="s" s="2">
         <v>458</v>
@@ -24660,7 +24657,7 @@
     </row>
     <row r="194">
       <c r="A194" t="s" s="2">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B194" t="s" s="2">
         <v>459</v>
@@ -24776,7 +24773,7 @@
     </row>
     <row r="195">
       <c r="A195" t="s" s="2">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B195" t="s" s="2">
         <v>478</v>
@@ -24888,7 +24885,7 @@
     </row>
     <row r="196">
       <c r="A196" t="s" s="2">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B196" t="s" s="2">
         <v>480</v>
@@ -25002,7 +24999,7 @@
     </row>
     <row r="197">
       <c r="A197" t="s" s="2">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B197" t="s" s="2">
         <v>482</v>
@@ -25118,7 +25115,7 @@
     </row>
     <row r="198">
       <c r="A198" t="s" s="2">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B198" t="s" s="2">
         <v>491</v>
@@ -25163,7 +25160,7 @@
       </c>
       <c r="Q198" s="2"/>
       <c r="R198" t="s" s="2">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="S198" t="s" s="2">
         <v>76</v>
@@ -25234,7 +25231,7 @@
     </row>
     <row r="199">
       <c r="A199" t="s" s="2">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B199" t="s" s="2">
         <v>466</v>
@@ -25263,7 +25260,7 @@
         <v>252</v>
       </c>
       <c r="L199" t="s" s="2">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="M199" t="s" s="2">
         <v>469</v>
@@ -25297,7 +25294,7 @@
       </c>
       <c r="Y199" s="2"/>
       <c r="Z199" t="s" s="2">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AA199" t="s" s="2">
         <v>76</v>
@@ -25344,13 +25341,13 @@
     </row>
     <row r="200">
       <c r="A200" t="s" s="2">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B200" t="s" s="2">
         <v>448</v>
       </c>
       <c r="C200" t="s" s="2">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D200" t="s" s="2">
         <v>449</v>
@@ -25375,7 +25372,7 @@
         <v>418</v>
       </c>
       <c r="L200" t="s" s="2">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="M200" t="s" s="2">
         <v>452</v>
@@ -25460,7 +25457,7 @@
     </row>
     <row r="201">
       <c r="A201" t="s" s="2">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B201" t="s" s="2">
         <v>456</v>
@@ -25572,7 +25569,7 @@
     </row>
     <row r="202">
       <c r="A202" t="s" s="2">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B202" t="s" s="2">
         <v>457</v>
@@ -25686,7 +25683,7 @@
     </row>
     <row r="203">
       <c r="A203" t="s" s="2">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B203" t="s" s="2">
         <v>458</v>
@@ -25802,7 +25799,7 @@
     </row>
     <row r="204">
       <c r="A204" t="s" s="2">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B204" t="s" s="2">
         <v>459</v>
@@ -25918,7 +25915,7 @@
     </row>
     <row r="205">
       <c r="A205" t="s" s="2">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B205" t="s" s="2">
         <v>478</v>
@@ -26030,7 +26027,7 @@
     </row>
     <row r="206">
       <c r="A206" t="s" s="2">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B206" t="s" s="2">
         <v>480</v>
@@ -26144,7 +26141,7 @@
     </row>
     <row r="207">
       <c r="A207" t="s" s="2">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B207" t="s" s="2">
         <v>482</v>
@@ -26260,7 +26257,7 @@
     </row>
     <row r="208">
       <c r="A208" t="s" s="2">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B208" t="s" s="2">
         <v>491</v>
@@ -26305,7 +26302,7 @@
       </c>
       <c r="Q208" s="2"/>
       <c r="R208" t="s" s="2">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="S208" t="s" s="2">
         <v>76</v>
@@ -26376,7 +26373,7 @@
     </row>
     <row r="209">
       <c r="A209" t="s" s="2">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B209" t="s" s="2">
         <v>466</v>
@@ -26439,7 +26436,7 @@
       </c>
       <c r="Y209" s="2"/>
       <c r="Z209" t="s" s="2">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="AA209" t="s" s="2">
         <v>76</v>
@@ -26486,13 +26483,13 @@
     </row>
     <row r="210">
       <c r="A210" t="s" s="2">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B210" t="s" s="2">
         <v>448</v>
       </c>
       <c r="C210" t="s" s="2">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D210" t="s" s="2">
         <v>449</v>
@@ -26517,7 +26514,7 @@
         <v>418</v>
       </c>
       <c r="L210" t="s" s="2">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="M210" t="s" s="2">
         <v>452</v>
@@ -26602,7 +26599,7 @@
     </row>
     <row r="211">
       <c r="A211" t="s" s="2">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B211" t="s" s="2">
         <v>456</v>
@@ -26714,7 +26711,7 @@
     </row>
     <row r="212">
       <c r="A212" t="s" s="2">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B212" t="s" s="2">
         <v>457</v>
@@ -26828,7 +26825,7 @@
     </row>
     <row r="213">
       <c r="A213" t="s" s="2">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B213" t="s" s="2">
         <v>458</v>
@@ -26944,7 +26941,7 @@
     </row>
     <row r="214">
       <c r="A214" t="s" s="2">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B214" t="s" s="2">
         <v>459</v>
@@ -27060,7 +27057,7 @@
     </row>
     <row r="215">
       <c r="A215" t="s" s="2">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B215" t="s" s="2">
         <v>478</v>
@@ -27172,7 +27169,7 @@
     </row>
     <row r="216">
       <c r="A216" t="s" s="2">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B216" t="s" s="2">
         <v>480</v>
@@ -27286,7 +27283,7 @@
     </row>
     <row r="217">
       <c r="A217" t="s" s="2">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B217" t="s" s="2">
         <v>482</v>
@@ -27402,7 +27399,7 @@
     </row>
     <row r="218">
       <c r="A218" t="s" s="2">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B218" t="s" s="2">
         <v>491</v>
@@ -27447,7 +27444,7 @@
       </c>
       <c r="Q218" s="2"/>
       <c r="R218" t="s" s="2">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="S218" t="s" s="2">
         <v>76</v>
@@ -27518,7 +27515,7 @@
     </row>
     <row r="219">
       <c r="A219" t="s" s="2">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B219" t="s" s="2">
         <v>466</v>
@@ -27630,13 +27627,13 @@
     </row>
     <row r="220">
       <c r="A220" t="s" s="2">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B220" t="s" s="2">
         <v>448</v>
       </c>
       <c r="C220" t="s" s="2">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D220" t="s" s="2">
         <v>449</v>
@@ -27661,7 +27658,7 @@
         <v>418</v>
       </c>
       <c r="L220" t="s" s="2">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="M220" t="s" s="2">
         <v>452</v>
@@ -27746,7 +27743,7 @@
     </row>
     <row r="221">
       <c r="A221" t="s" s="2">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B221" t="s" s="2">
         <v>456</v>
@@ -27858,7 +27855,7 @@
     </row>
     <row r="222">
       <c r="A222" t="s" s="2">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B222" t="s" s="2">
         <v>457</v>
@@ -27972,7 +27969,7 @@
     </row>
     <row r="223">
       <c r="A223" t="s" s="2">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B223" t="s" s="2">
         <v>458</v>
@@ -28088,7 +28085,7 @@
     </row>
     <row r="224">
       <c r="A224" t="s" s="2">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B224" t="s" s="2">
         <v>459</v>
@@ -28204,7 +28201,7 @@
     </row>
     <row r="225">
       <c r="A225" t="s" s="2">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B225" t="s" s="2">
         <v>478</v>
@@ -28316,7 +28313,7 @@
     </row>
     <row r="226">
       <c r="A226" t="s" s="2">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B226" t="s" s="2">
         <v>480</v>
@@ -28430,7 +28427,7 @@
     </row>
     <row r="227">
       <c r="A227" t="s" s="2">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B227" t="s" s="2">
         <v>482</v>
@@ -28546,7 +28543,7 @@
     </row>
     <row r="228">
       <c r="A228" t="s" s="2">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B228" t="s" s="2">
         <v>491</v>
@@ -28591,7 +28588,7 @@
       </c>
       <c r="Q228" s="2"/>
       <c r="R228" t="s" s="2">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="S228" t="s" s="2">
         <v>76</v>
@@ -28662,7 +28659,7 @@
     </row>
     <row r="229">
       <c r="A229" t="s" s="2">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B229" t="s" s="2">
         <v>466</v>
@@ -28774,10 +28771,10 @@
     </row>
     <row r="230">
       <c r="A230" t="s" s="2">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B230" t="s" s="2">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C230" s="2"/>
       <c r="D230" t="s" s="2">
@@ -28803,14 +28800,14 @@
         <v>418</v>
       </c>
       <c r="L230" t="s" s="2">
+        <v>704</v>
+      </c>
+      <c r="M230" t="s" s="2">
         <v>705</v>
-      </c>
-      <c r="M230" t="s" s="2">
-        <v>706</v>
       </c>
       <c r="N230" s="2"/>
       <c r="O230" t="s" s="2">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="P230" t="s" s="2">
         <v>76</v>
@@ -28859,7 +28856,7 @@
         <v>76</v>
       </c>
       <c r="AF230" t="s" s="2">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="AG230" t="s" s="2">
         <v>77</v>
@@ -28888,10 +28885,10 @@
     </row>
     <row r="231">
       <c r="A231" t="s" s="2">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B231" t="s" s="2">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C231" s="2"/>
       <c r="D231" t="s" s="2">
@@ -29000,10 +28997,10 @@
     </row>
     <row r="232">
       <c r="A232" t="s" s="2">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B232" t="s" s="2">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C232" s="2"/>
       <c r="D232" t="s" s="2">
@@ -29114,10 +29111,10 @@
     </row>
     <row r="233">
       <c r="A233" t="s" s="2">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B233" t="s" s="2">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C233" s="2"/>
       <c r="D233" t="s" s="2">
@@ -29230,10 +29227,10 @@
     </row>
     <row r="234">
       <c r="A234" t="s" s="2">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B234" t="s" s="2">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C234" s="2"/>
       <c r="D234" t="s" s="2">
@@ -29259,16 +29256,16 @@
         <v>252</v>
       </c>
       <c r="L234" t="s" s="2">
+        <v>711</v>
+      </c>
+      <c r="M234" t="s" s="2">
         <v>712</v>
-      </c>
-      <c r="M234" t="s" s="2">
-        <v>713</v>
       </c>
       <c r="N234" t="s" s="2">
         <v>262</v>
       </c>
       <c r="O234" t="s" s="2">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="P234" t="s" s="2">
         <v>76</v>
@@ -29296,7 +29293,7 @@
         <v>156</v>
       </c>
       <c r="Y234" t="s" s="2">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="Z234" t="s" s="2">
         <v>76</v>
@@ -29317,7 +29314,7 @@
         <v>76</v>
       </c>
       <c r="AF234" t="s" s="2">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="AG234" t="s" s="2">
         <v>86</v>
@@ -29346,10 +29343,10 @@
     </row>
     <row r="235">
       <c r="A235" t="s" s="2">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B235" t="s" s="2">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C235" s="2"/>
       <c r="D235" t="s" s="2">
@@ -29375,14 +29372,14 @@
         <v>467</v>
       </c>
       <c r="L235" t="s" s="2">
+        <v>716</v>
+      </c>
+      <c r="M235" t="s" s="2">
         <v>717</v>
-      </c>
-      <c r="M235" t="s" s="2">
-        <v>718</v>
       </c>
       <c r="N235" s="2"/>
       <c r="O235" t="s" s="2">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="P235" t="s" s="2">
         <v>76</v>
@@ -29431,7 +29428,7 @@
         <v>76</v>
       </c>
       <c r="AF235" t="s" s="2">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="AG235" t="s" s="2">
         <v>86</v>

</xml_diff>